<commit_message>
Improve the code and dependent libraries
</commit_message>
<xml_diff>
--- a/DemoAPI/data/DemoAPITestCase_bak.xlsx
+++ b/DemoAPI/data/DemoAPITestCase_bak.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitproject\automation_interface\DemoAPI\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD30B708-A28E-4B15-8B5E-B44750BAD5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="390" windowWidth="27795" windowHeight="12045"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -294,7 +300,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -432,6 +438,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -479,7 +488,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -512,9 +521,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -547,6 +573,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -722,7 +765,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1358,24 +1401,24 @@
       <c r="C33" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M15"/>
+  <autoFilter ref="A1:M15" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D7" r:id="rId6"/>
-    <hyperlink ref="D8" r:id="rId7"/>
-    <hyperlink ref="D9" r:id="rId8"/>
-    <hyperlink ref="D10" r:id="rId9"/>
-    <hyperlink ref="D11" r:id="rId10"/>
-    <hyperlink ref="D12" r:id="rId11"/>
-    <hyperlink ref="D13" r:id="rId12"/>
-    <hyperlink ref="D14" r:id="rId13"/>
-    <hyperlink ref="D15" r:id="rId14"/>
-    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
@@ -1383,7 +1426,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1396,7 +1439,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>